<commit_message>
Add updated base BOM
Now includes most RF components and SMDs.
</commit_message>
<xml_diff>
--- a/specs/base-bom.xlsx
+++ b/specs/base-bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="136">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -140,9 +140,6 @@
     <t>712-CONSMA001-SMD-G</t>
   </si>
   <si>
-    <t>Linx Technologies</t>
-  </si>
-  <si>
     <t>IRLML2502TRPBF</t>
   </si>
   <si>
@@ -284,9 +281,6 @@
     <t>SMT0603</t>
   </si>
   <si>
-    <t>Murata Electronics</t>
-  </si>
-  <si>
     <t>Total per unit</t>
   </si>
   <si>
@@ -302,9 +296,6 @@
     <t>4-SMD</t>
   </si>
   <si>
-    <t>!!!</t>
-  </si>
-  <si>
     <t>SMT0805</t>
   </si>
   <si>
@@ -356,19 +347,101 @@
     <t>4.7uF</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>GRM155R61A105KE01D</t>
+  </si>
+  <si>
+    <t>AE2-1</t>
+  </si>
+  <si>
+    <t>AE2-2</t>
+  </si>
+  <si>
+    <t>0 Ohm</t>
+  </si>
+  <si>
+    <t>RCS04020000Z0ED</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>Linx</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>ANT-916-PML</t>
+  </si>
+  <si>
+    <t>Half-Wave Whip</t>
+  </si>
+  <si>
+    <t>916MHz</t>
+  </si>
+  <si>
+    <t>Newark</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>SMA Straight Plug</t>
+  </si>
+  <si>
+    <t>RCS0402100RFKED</t>
+  </si>
+  <si>
+    <t>RCS04021K00FKED</t>
+  </si>
+  <si>
+    <t>RCS040210K0FKED</t>
+  </si>
+  <si>
+    <t>RCS0402100KFKED</t>
+  </si>
+  <si>
+    <t>36401E9N1ATDF</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>CV201210-4R7K</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>GRM155R61H104JE14D</t>
+  </si>
+  <si>
+    <t>GRM155R71H103JA88D</t>
+  </si>
+  <si>
+    <t>GRM1555C1H470FA01D</t>
+  </si>
+  <si>
+    <t>GRM155R61A225KE95D</t>
+  </si>
+  <si>
+    <t>04026D475KAT2A</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>GRM155C80J106ME11D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -415,7 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -442,6 +515,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -723,18 +798,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
@@ -756,10 +829,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
@@ -791,10 +864,10 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="D2" s="7"/>
       <c r="F2" s="7">
@@ -830,10 +903,10 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="D3" s="7"/>
       <c r="F3" s="7">
@@ -869,10 +942,10 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="D4" s="7"/>
       <c r="F4" s="7">
@@ -908,10 +981,10 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="D5" s="7"/>
       <c r="F5" s="7">
@@ -947,10 +1020,10 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="D6" s="7"/>
       <c r="F6" s="7">
@@ -983,10 +1056,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -1006,10 +1076,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
@@ -1029,10 +1096,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
@@ -1052,10 +1116,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="F10" s="7">
         <v>1</v>
@@ -1075,10 +1136,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="F11" s="7">
         <v>1</v>
@@ -1098,10 +1156,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="F12" s="7">
         <v>1</v>
@@ -1121,10 +1176,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="F13" s="7">
         <v>1</v>
@@ -1144,10 +1196,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="F14" s="7">
         <v>1</v>
@@ -1167,10 +1216,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="F15" s="7">
         <v>1</v>
@@ -1190,19 +1236,19 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F16" s="7">
         <v>1</v>
@@ -1234,204 +1280,327 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F17" s="7">
         <v>1</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.1</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1.4E-2</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="L17" s="4">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" t="s">
+        <v>112</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
       </c>
+      <c r="G18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I18" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="I18:I19" si="3">$F18*H18</f>
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1.4E-2</v>
       </c>
       <c r="K18" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="K18:K19" si="4">$F18*J18*50</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="L18" s="4">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="M18:M19" si="5">$F18*L18*100</f>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F19" s="7">
         <v>1</v>
       </c>
+      <c r="G19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I19" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1.4E-2</v>
       </c>
       <c r="K19" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="L19" s="4">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>133</v>
       </c>
       <c r="C20" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F20" s="7">
         <v>1</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.13</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.13</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.115</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.75</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.104</v>
       </c>
       <c r="M20" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" t="s">
+        <v>112</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F21" s="7">
         <v>1</v>
       </c>
+      <c r="G21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="I21" si="6">$F21*H21</f>
+        <v>0.1</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1.4E-2</v>
       </c>
       <c r="K21" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="K21" si="7">$F21*J21*50</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="L21" s="12">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="M21" si="8">$F21*L21*100</f>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F22" s="7">
         <v>1</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.1</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.06</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="L22" s="4">
+        <v>2.7E-2</v>
       </c>
       <c r="M22" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" t="s">
+        <v>112</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F23" s="7">
         <v>1</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.1</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="J23" s="4">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="L23" s="4">
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="M23" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F24" s="7">
         <v>1</v>
@@ -1463,19 +1632,19 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F25" s="7">
         <v>1</v>
@@ -1507,19 +1676,19 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F26" s="7">
         <v>1</v>
@@ -1551,45 +1720,63 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" t="s">
+        <v>112</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F27" s="7">
         <v>1</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.1</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="J27" s="4">
+        <v>2.3E-2</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L27" s="4">
+        <v>1.6E-2</v>
       </c>
       <c r="M27" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F28" s="7">
         <v>1</v>
@@ -1621,28 +1808,46 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F29" s="7">
         <v>1</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.16</v>
       </c>
       <c r="I29" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16</v>
+      </c>
+      <c r="J29" s="4">
+        <v>6.2E-2</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.1</v>
+      </c>
+      <c r="L29" s="4">
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="M29" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1686,16 +1891,16 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F31" s="7">
         <v>1</v>
@@ -1727,7 +1932,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F32" s="7">
         <v>1</v>
@@ -1747,7 +1952,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F33" s="7">
         <v>1</v>
@@ -1767,159 +1972,189 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F34" s="7">
         <v>1</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" ref="I34:I65" si="3">$F34*H34</f>
+        <f t="shared" ref="I34:I54" si="9">$F34*H34</f>
         <v>0</v>
       </c>
       <c r="K34" s="5">
-        <f t="shared" ref="K34:K65" si="4">$F34*J34*50</f>
+        <f t="shared" ref="K34:K54" si="10">$F34*J34*50</f>
         <v>0</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" ref="M34:M65" si="5">$F34*L34*100</f>
+        <f t="shared" ref="M34:M54" si="11">$F34*L34*100</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F35" s="7">
         <v>1</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K35" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M35" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" t="s">
+        <v>126</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F36" s="7">
         <v>1</v>
       </c>
+      <c r="G36" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I36" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>0.1</v>
+      </c>
+      <c r="J36" s="4">
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="K36" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.55</v>
+      </c>
+      <c r="L36" s="4">
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="M36" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>6.1</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" t="s">
+        <v>128</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F37" s="7">
         <v>1</v>
       </c>
+      <c r="G37" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I37" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>0.1</v>
+      </c>
+      <c r="J37" s="4">
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="K37" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>2.4</v>
+      </c>
+      <c r="L37" s="4">
+        <v>3.9E-2</v>
       </c>
       <c r="M37" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>3.9</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K38" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F39" s="7">
         <v>1</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K39" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M39" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F40" s="7">
         <v>1</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K40" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M40" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -1928,13 +2163,13 @@
         <v>30</v>
       </c>
       <c r="B41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="D41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F41" s="7">
         <v>1</v>
@@ -1946,174 +2181,264 @@
         <v>0.46</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.46</v>
       </c>
       <c r="J41" s="5">
         <v>0.32900000000000001</v>
       </c>
       <c r="K41" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>16.45</v>
       </c>
       <c r="L41" s="1">
         <v>0.151</v>
       </c>
       <c r="M41" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>15.1</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" t="s">
+        <v>114</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="E42" t="s">
+        <v>110</v>
       </c>
       <c r="F42" s="7">
         <v>1</v>
       </c>
+      <c r="G42" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I42" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>0.1</v>
+      </c>
+      <c r="J42" s="12">
+        <v>4.9200000000000001E-2</v>
       </c>
       <c r="K42" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>2.46</v>
+      </c>
+      <c r="L42" s="12">
+        <v>3.5200000000000002E-2</v>
       </c>
       <c r="M42" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>3.52</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" t="s">
+        <v>114</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F43" s="7">
         <v>1</v>
       </c>
+      <c r="G43" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0.11</v>
+      </c>
       <c r="I43" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0.11</v>
       </c>
       <c r="K43" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>5.5</v>
+      </c>
+      <c r="L43" s="4">
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M43" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>3.8</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" t="s">
+        <v>114</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E44" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F44" s="7">
         <v>1</v>
       </c>
+      <c r="G44" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.11</v>
+      </c>
       <c r="I44" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="I44" si="12">$F44*H44</f>
+        <v>0.11</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.11</v>
       </c>
       <c r="K44" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="K44" si="13">$F44*J44*50</f>
+        <v>5.5</v>
+      </c>
+      <c r="L44" s="4">
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M44" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" ref="M44" si="14">$F44*L44*100</f>
+        <v>3.8</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="B45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" t="s">
+        <v>114</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E45" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F45" s="7">
         <v>1</v>
       </c>
+      <c r="G45" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.11</v>
+      </c>
       <c r="I45" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.11</v>
       </c>
       <c r="K45" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>5.5</v>
+      </c>
+      <c r="L45" s="4">
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M45" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>3.8</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="B46" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" t="s">
+        <v>114</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F46" s="7">
         <v>1</v>
       </c>
+      <c r="G46" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0.11</v>
+      </c>
       <c r="I46" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="I46" si="15">$F46*H46</f>
+        <v>0.11</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.11</v>
       </c>
       <c r="K46" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="K46" si="16">$F46*J46*50</f>
+        <v>5.5</v>
+      </c>
+      <c r="L46" s="4">
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M46" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" ref="M46" si="17">$F46*L46*100</f>
+        <v>3.8</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E47" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F47" s="7">
         <v>1</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K47" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -2125,7 +2450,7 @@
         <v>37</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="D48" s="7"/>
       <c r="F48" s="7">
@@ -2138,25 +2463,25 @@
         <v>2.86</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.86</v>
       </c>
       <c r="J48" s="5">
         <v>2.59</v>
       </c>
       <c r="K48" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>129.5</v>
       </c>
       <c r="L48" s="1">
         <v>2.4700000000000002</v>
       </c>
       <c r="M48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>247.00000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>11</v>
       </c>
@@ -2167,7 +2492,7 @@
         <v>8</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F49" s="7">
         <v>1</v>
@@ -2179,25 +2504,25 @@
         <v>3.51</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.51</v>
       </c>
       <c r="J49" s="5">
         <v>3.21</v>
       </c>
       <c r="K49" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>160.5</v>
       </c>
       <c r="L49" s="5">
         <v>3.02</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>302</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>14</v>
       </c>
@@ -2217,28 +2542,25 @@
         <v>39</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>39</v>
       </c>
       <c r="J50" s="5">
         <v>39</v>
       </c>
       <c r="K50" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1950</v>
       </c>
       <c r="L50" s="5">
         <v>39</v>
       </c>
       <c r="M50" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>3900</v>
       </c>
-      <c r="N50" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
@@ -2249,10 +2571,10 @@
         <v>22</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F51" s="7">
         <v>1</v>
@@ -2264,25 +2586,25 @@
         <v>0.71</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.71</v>
       </c>
       <c r="J51" s="5">
         <v>3.21</v>
       </c>
       <c r="K51" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>160.5</v>
       </c>
       <c r="L51" s="5">
         <v>0.51619999999999999</v>
       </c>
       <c r="M51" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>51.62</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>13</v>
       </c>
@@ -2293,10 +2615,10 @@
         <v>24</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F52" s="7">
         <v>1</v>
@@ -2308,56 +2630,141 @@
         <v>0.76</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.76</v>
       </c>
       <c r="J52" s="5">
         <v>0.66300000000000003</v>
       </c>
       <c r="K52" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>33.15</v>
       </c>
       <c r="L52" s="5">
         <v>0.56000000000000005</v>
       </c>
       <c r="M52" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F53" s="7">
+        <v>1</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="1">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="I53" s="1">
+        <f t="shared" si="9"/>
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="J53" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="K53" s="1">
+        <f t="shared" si="10"/>
+        <v>375</v>
+      </c>
+      <c r="L53" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="M53" s="1">
+        <f t="shared" si="11"/>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" s="13">
+        <v>132193</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F54" s="7">
+        <v>1</v>
+      </c>
       <c r="G54" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H54" s="1">
+        <v>6.12</v>
+      </c>
+      <c r="I54" s="1">
+        <f t="shared" si="9"/>
+        <v>6.12</v>
+      </c>
+      <c r="J54" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="K54" s="1">
+        <f t="shared" si="10"/>
+        <v>254.99999999999997</v>
+      </c>
+      <c r="L54" s="1">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="M54" s="1">
+        <f t="shared" si="11"/>
+        <v>484.99999999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G56" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I54" s="1">
-        <f>SUM(I2:I52)</f>
-        <v>59.980000000000004</v>
-      </c>
-      <c r="K54" s="1">
-        <f>SUM(K2:K52)</f>
-        <v>2950.1</v>
-      </c>
-      <c r="M54" s="1">
-        <f>SUM(M2:M52)</f>
-        <v>5551.05</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G55" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I55" s="1">
-        <f>I54/1</f>
-        <v>59.980000000000004</v>
-      </c>
-      <c r="K55" s="1">
-        <f>K54/50</f>
-        <v>59.001999999999995</v>
-      </c>
-      <c r="M55" s="1">
-        <f>M54/100</f>
-        <v>55.5105</v>
+      <c r="I56" s="1">
+        <f>SUM(I2:I54)</f>
+        <v>75.95</v>
+      </c>
+      <c r="K56" s="1">
+        <f>SUM(K2:K54)</f>
+        <v>3626.76</v>
+      </c>
+      <c r="M56" s="1">
+        <f>SUM(M2:M54)</f>
+        <v>6777.97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G57" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I57" s="1">
+        <f>I56/1</f>
+        <v>75.95</v>
+      </c>
+      <c r="K57" s="1">
+        <f>K56/50</f>
+        <v>72.535200000000003</v>
+      </c>
+      <c r="M57" s="1">
+        <f>M56/100</f>
+        <v>67.779700000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix footprints for connectors and crystal
Unnecessary SMDs in the matching circuit and 0 ohm link removed from the
schematic. Certain resistor and capacitor values updated to new offical
BOM components.
</commit_message>
<xml_diff>
--- a/specs/base-bom.xlsx
+++ b/specs/base-bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzheng13\Documents\HA-HA\specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey Zheng\Dropbox\HA-HA\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="146">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -71,9 +71,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>DS1</t>
-  </si>
-  <si>
     <t>CFAH1604A-TMI-JT</t>
   </si>
   <si>
@@ -134,18 +131,9 @@
     <t>B5</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>712-CONSMA001-SMD-G</t>
-  </si>
-  <si>
     <t>IRLML2502TRPBF</t>
   </si>
   <si>
-    <t>Infineon Technologies</t>
-  </si>
-  <si>
     <t>KS-01Q-01</t>
   </si>
   <si>
@@ -356,12 +344,6 @@
     <t>AE2-2</t>
   </si>
   <si>
-    <t>0 Ohm</t>
-  </si>
-  <si>
-    <t>RCS04020000Z0ED</t>
-  </si>
-  <si>
     <t>Murata</t>
   </si>
   <si>
@@ -374,9 +356,6 @@
     <t>ANT-916-PML</t>
   </si>
   <si>
-    <t>Half-Wave Whip</t>
-  </si>
-  <si>
     <t>916MHz</t>
   </si>
   <si>
@@ -386,18 +365,12 @@
     <t>Amphenol</t>
   </si>
   <si>
-    <t>SMA Straight Plug</t>
-  </si>
-  <si>
     <t>RCS0402100RFKED</t>
   </si>
   <si>
     <t>RCS04021K00FKED</t>
   </si>
   <si>
-    <t>RCS040210K0FKED</t>
-  </si>
-  <si>
     <t>RCS0402100KFKED</t>
   </si>
   <si>
@@ -432,6 +405,63 @@
   </si>
   <si>
     <t>GRM155C80J106ME11D</t>
+  </si>
+  <si>
+    <t>DS1-2</t>
+  </si>
+  <si>
+    <t>DS1-3</t>
+  </si>
+  <si>
+    <t>DS1-1</t>
+  </si>
+  <si>
+    <t>16x4</t>
+  </si>
+  <si>
+    <t>PREC016SAAN-RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sullins </t>
+  </si>
+  <si>
+    <t>Infineon</t>
+  </si>
+  <si>
+    <t>302-R201</t>
+  </si>
+  <si>
+    <t>On Shore</t>
+  </si>
+  <si>
+    <t>310-87-116-41-001101</t>
+  </si>
+  <si>
+    <t>Preci-Dip</t>
+  </si>
+  <si>
+    <t>3309W-1-103</t>
+  </si>
+  <si>
+    <t>OSTTE020104</t>
+  </si>
+  <si>
+    <t>OSTTE020105</t>
+  </si>
+  <si>
+    <t>OSTTE020106</t>
+  </si>
+  <si>
+    <t>Arrow</t>
+  </si>
+  <si>
+    <t>10pF</t>
+  </si>
+  <si>
+    <t>GRM1555C1H100FA01D</t>
+  </si>
+  <si>
+    <t>SMT0403</t>
   </si>
 </sst>
 </file>
@@ -798,7 +828,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -829,10 +859,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
@@ -844,76 +874,76 @@
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D2" s="7"/>
       <c r="F2" s="7">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1">
         <v>0.52</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I33" si="0">$F2*H2</f>
+        <f t="shared" ref="I2:I32" si="0">$F2*H2</f>
         <v>0.52</v>
       </c>
       <c r="J2" s="5">
         <v>0.44700000000000001</v>
       </c>
       <c r="K2" s="5">
-        <f t="shared" ref="K2:K33" si="1">$F2*J2*50</f>
+        <f t="shared" ref="K2:K32" si="1">$F2*J2*50</f>
         <v>22.35</v>
       </c>
       <c r="L2" s="1">
         <v>0.435</v>
       </c>
       <c r="M2" s="1">
-        <f t="shared" ref="M2:M33" si="2">$F2*L2*100</f>
+        <f t="shared" ref="M2:M32" si="2">$F2*L2*100</f>
         <v>43.5</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D3" s="7"/>
       <c r="F3" s="7">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1">
         <v>0.52</v>
@@ -939,20 +969,20 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D4" s="7"/>
       <c r="F4" s="7">
         <v>1</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="1">
         <v>0.52</v>
@@ -978,20 +1008,20 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D5" s="7"/>
       <c r="F5" s="7">
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="1">
         <v>0.52</v>
@@ -1017,20 +1047,20 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D6" s="7"/>
       <c r="F6" s="7">
         <v>1</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1">
         <v>0.52</v>
@@ -1056,11 +1086,9 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F7" s="7"/>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1076,11 +1104,9 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F8" s="7"/>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1096,11 +1122,9 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="7">
-        <v>1</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F9" s="7"/>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1116,11 +1140,9 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="7">
-        <v>1</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F10" s="7"/>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1136,11 +1158,9 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F11" s="7"/>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1156,11 +1176,9 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="7">
-        <v>1</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F12" s="7"/>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1176,11 +1194,9 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="7">
-        <v>1</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F13" s="7"/>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1196,65 +1212,113 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" t="s">
+        <v>143</v>
       </c>
       <c r="F14" s="7">
         <v>1</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.1</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="4">
+        <v>2.3E-2</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1.6E-2</v>
       </c>
       <c r="M14" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" t="s">
+        <v>143</v>
       </c>
       <c r="F15" s="7">
         <v>1</v>
       </c>
+      <c r="G15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I15" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="I15" si="3">$F15*H15</f>
+        <v>0.1</v>
+      </c>
+      <c r="J15" s="4">
+        <v>2.3E-2</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="K15" si="4">$F15*J15*50</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1.6E-2</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="M15" si="5">$F15*L15*100</f>
+        <v>1.6</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F16" s="7">
         <v>1</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="1">
         <v>0.1</v>
@@ -1280,25 +1344,25 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F17" s="7">
         <v>1</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="1">
         <v>0.1</v>
@@ -1324,113 +1388,113 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H18" s="1">
         <v>0.1</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" ref="I18:I19" si="3">$F18*H18</f>
+        <f t="shared" ref="I18:I19" si="6">$F18*H18</f>
         <v>0.1</v>
       </c>
       <c r="J18" s="4">
         <v>1.4E-2</v>
       </c>
       <c r="K18" s="5">
-        <f t="shared" ref="K18:K19" si="4">$F18*J18*50</f>
+        <f t="shared" ref="K18:K19" si="7">$F18*J18*50</f>
         <v>0.70000000000000007</v>
       </c>
       <c r="L18" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" ref="M18:M19" si="5">$F18*L18*100</f>
+        <f t="shared" ref="M18:M19" si="8">$F18*L18*100</f>
         <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F19" s="7">
         <v>1</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
       <c r="J19" s="4">
         <v>1.4E-2</v>
       </c>
       <c r="K19" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.70000000000000007</v>
       </c>
       <c r="L19" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C20" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F20" s="7">
         <v>1</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H20" s="1">
         <v>0.13</v>
@@ -1456,69 +1520,69 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F21" s="7">
         <v>1</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H21" s="1">
         <v>0.1</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" ref="I21" si="6">$F21*H21</f>
+        <f t="shared" ref="I21" si="9">$F21*H21</f>
         <v>0.1</v>
       </c>
       <c r="J21" s="4">
         <v>1.4E-2</v>
       </c>
       <c r="K21" s="5">
-        <f t="shared" ref="K21" si="7">$F21*J21*50</f>
+        <f t="shared" ref="K21" si="10">$F21*J21*50</f>
         <v>0.70000000000000007</v>
       </c>
       <c r="L21" s="12">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" ref="M21" si="8">$F21*L21*100</f>
+        <f t="shared" ref="M21" si="11">$F21*L21*100</f>
         <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F22" s="7">
         <v>1</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H22" s="1">
         <v>0.1</v>
@@ -1544,25 +1608,25 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F23" s="7">
         <v>1</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H23" s="1">
         <v>0.1</v>
@@ -1588,25 +1652,25 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E24" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F24" s="7">
         <v>1</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H24" s="1">
         <v>0.1</v>
@@ -1632,25 +1696,25 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F25" s="7">
         <v>1</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H25" s="1">
         <v>0.1</v>
@@ -1676,25 +1740,25 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F26" s="7">
         <v>1</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H26" s="1">
         <v>0.1</v>
@@ -1720,25 +1784,25 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F27" s="7">
         <v>1</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H27" s="1">
         <v>0.1</v>
@@ -1764,25 +1828,25 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E28" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F28" s="7">
         <v>1</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H28" s="1">
         <v>0.1</v>
@@ -1808,25 +1872,25 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F29" s="7">
         <v>1</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H29" s="1">
         <v>0.16</v>
@@ -1852,20 +1916,23 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="D30" s="7"/>
+      <c r="E30" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="F30" s="7">
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" s="5">
         <v>9.48</v>
@@ -1891,880 +1958,973 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>84</v>
+        <v>132</v>
       </c>
       <c r="F31" s="7">
         <v>1</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H31" s="1">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="J31" s="1">
-        <v>0.05</v>
+        <v>0.3</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0.27200000000000002</v>
       </c>
       <c r="K31" s="5">
         <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="L31" s="1">
-        <v>4.3299999999999998E-2</v>
+        <v>13.600000000000001</v>
+      </c>
+      <c r="L31" s="12">
+        <v>0.22389999999999999</v>
       </c>
       <c r="M31" s="1">
         <f t="shared" si="2"/>
-        <v>4.33</v>
+        <v>22.39</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>42</v>
+        <v>128</v>
+      </c>
+      <c r="B32" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" t="s">
+        <v>137</v>
       </c>
       <c r="F32" s="7">
         <v>1</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0.91</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.91</v>
+      </c>
+      <c r="J32" s="4">
+        <v>0.79600000000000004</v>
       </c>
       <c r="K32" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>39.800000000000004</v>
+      </c>
+      <c r="L32" s="12">
+        <v>0.68659999999999999</v>
       </c>
       <c r="M32" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>68.66</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="F33" s="7">
         <v>1</v>
       </c>
+      <c r="G33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I33" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="I33:I40" si="12">$F33*H33</f>
+        <v>0.1</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.05</v>
       </c>
       <c r="K33" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="K33:K40" si="13">$F33*J33*50</f>
+        <v>2.5</v>
+      </c>
+      <c r="L33" s="1">
+        <v>4.3299999999999998E-2</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="M33:M40" si="14">$F33*L33*100</f>
+        <v>4.33</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>73</v>
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" t="s">
+        <v>135</v>
       </c>
       <c r="F34" s="7">
         <v>1</v>
       </c>
+      <c r="G34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.62</v>
+      </c>
       <c r="I34" s="1">
-        <f t="shared" ref="I34:I54" si="9">$F34*H34</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0.62</v>
+      </c>
+      <c r="J34" s="12">
+        <v>0.4632</v>
       </c>
       <c r="K34" s="5">
-        <f t="shared" ref="K34:K54" si="10">$F34*J34*50</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>23.16</v>
+      </c>
+      <c r="L34" s="12">
+        <v>0.44390000000000002</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" ref="M34:M54" si="11">$F34*L34*100</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>44.39</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" s="7">
-        <v>1</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F35" s="7"/>
       <c r="I35" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K35" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M35" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" t="s">
-        <v>125</v>
-      </c>
-      <c r="C36" t="s">
-        <v>126</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" t="s">
-        <v>97</v>
-      </c>
-      <c r="F36" s="7">
-        <v>1</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0.1</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F36" s="7"/>
       <c r="I36" s="1">
-        <f t="shared" si="9"/>
-        <v>0.1</v>
-      </c>
-      <c r="J36" s="4">
-        <v>7.0999999999999994E-2</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="K36" s="5">
-        <f t="shared" si="10"/>
-        <v>3.55</v>
-      </c>
-      <c r="L36" s="4">
-        <v>6.0999999999999999E-2</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="M36" s="1">
-        <f t="shared" si="11"/>
-        <v>6.1</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" t="s">
-        <v>127</v>
-      </c>
-      <c r="C37" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E37" t="s">
-        <v>98</v>
-      </c>
-      <c r="F37" s="7">
-        <v>1</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="1">
-        <v>0.1</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="F37" s="7"/>
       <c r="I37" s="1">
-        <f t="shared" si="9"/>
-        <v>0.1</v>
-      </c>
-      <c r="J37" s="4">
-        <v>4.8000000000000001E-2</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="K37" s="5">
-        <f t="shared" si="10"/>
-        <v>2.4</v>
-      </c>
-      <c r="L37" s="4">
-        <v>3.9E-2</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="M37" s="1">
-        <f t="shared" si="11"/>
-        <v>3.9</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" t="s">
+        <v>93</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
       </c>
+      <c r="G38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I38" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0.1</v>
+      </c>
+      <c r="J38" s="4">
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="K38" s="5">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>3.55</v>
+      </c>
+      <c r="L38" s="4">
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="M38" s="1">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>6.1</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" t="s">
+        <v>94</v>
       </c>
       <c r="F39" s="7">
         <v>1</v>
       </c>
+      <c r="G39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I39" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0.1</v>
+      </c>
+      <c r="J39" s="4">
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="K39" s="5">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>2.4</v>
+      </c>
+      <c r="L39" s="4">
+        <v>3.9E-2</v>
       </c>
       <c r="M39" s="1">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>3.9</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
+      </c>
+      <c r="B40" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" t="s">
+        <v>135</v>
       </c>
       <c r="F40" s="7">
         <v>1</v>
       </c>
+      <c r="G40" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="H40" s="12">
+        <v>0.34670000000000001</v>
+      </c>
       <c r="I40" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0.34670000000000001</v>
+      </c>
+      <c r="J40" s="12">
+        <v>0.2442</v>
       </c>
       <c r="K40" s="5">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>12.21</v>
+      </c>
+      <c r="L40" s="12">
+        <v>0.2442</v>
       </c>
       <c r="M40" s="1">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>24.42</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" t="s">
-        <v>86</v>
+        <v>140</v>
+      </c>
+      <c r="C41" t="s">
+        <v>135</v>
       </c>
       <c r="F41" s="7">
         <v>1</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="1">
-        <v>0.46</v>
+        <v>142</v>
+      </c>
+      <c r="H41" s="12">
+        <v>0.34670000000000001</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" si="9"/>
-        <v>0.46</v>
-      </c>
-      <c r="J41" s="5">
-        <v>0.32900000000000001</v>
+        <f t="shared" ref="I41:I42" si="15">$F41*H41</f>
+        <v>0.34670000000000001</v>
+      </c>
+      <c r="J41" s="12">
+        <v>0.2442</v>
       </c>
       <c r="K41" s="5">
-        <f t="shared" si="10"/>
-        <v>16.45</v>
-      </c>
-      <c r="L41" s="1">
-        <v>0.151</v>
+        <f t="shared" ref="K41:K42" si="16">$F41*J41*50</f>
+        <v>12.21</v>
+      </c>
+      <c r="L41" s="12">
+        <v>0.2442</v>
       </c>
       <c r="M41" s="1">
-        <f t="shared" si="11"/>
-        <v>15.1</v>
+        <f t="shared" ref="M41:M42" si="17">$F41*L41*100</f>
+        <v>24.42</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="C42" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="F42" s="7">
         <v>1</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H42" s="1">
-        <v>0.1</v>
+        <v>142</v>
+      </c>
+      <c r="H42" s="12">
+        <v>0.34670000000000001</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" si="9"/>
-        <v>0.1</v>
+        <f t="shared" si="15"/>
+        <v>0.34670000000000001</v>
       </c>
       <c r="J42" s="12">
-        <v>4.9200000000000001E-2</v>
+        <v>0.2442</v>
       </c>
       <c r="K42" s="5">
-        <f t="shared" si="10"/>
-        <v>2.46</v>
+        <f t="shared" si="16"/>
+        <v>12.21</v>
       </c>
       <c r="L42" s="12">
-        <v>3.5200000000000002E-2</v>
+        <v>0.2442</v>
       </c>
       <c r="M42" s="1">
-        <f t="shared" si="11"/>
-        <v>3.52</v>
+        <f t="shared" si="17"/>
+        <v>24.42</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E43" t="s">
-        <v>99</v>
+        <v>35</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D43" t="s">
+        <v>82</v>
       </c>
       <c r="F43" s="7">
         <v>1</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H43" s="1">
-        <v>0.11</v>
+        <v>0.46</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-      <c r="J43" s="1">
-        <v>0.11</v>
+        <f t="shared" ref="I43:I55" si="18">$F43*H43</f>
+        <v>0.46</v>
+      </c>
+      <c r="J43" s="5">
+        <v>0.32900000000000001</v>
       </c>
       <c r="K43" s="5">
-        <f t="shared" si="10"/>
-        <v>5.5</v>
-      </c>
-      <c r="L43" s="4">
-        <v>3.7999999999999999E-2</v>
+        <f t="shared" ref="K43:K55" si="19">$F43*J43*50</f>
+        <v>16.45</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0.151</v>
       </c>
       <c r="M43" s="1">
-        <f t="shared" si="11"/>
-        <v>3.8</v>
+        <f t="shared" ref="M43:M55" si="20">$F43*L43*100</f>
+        <v>15.1</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" t="s">
-        <v>124</v>
-      </c>
-      <c r="C44" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" t="s">
-        <v>100</v>
-      </c>
-      <c r="F44" s="7">
-        <v>1</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H44" s="1">
-        <v>0.11</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F44" s="7"/>
       <c r="I44" s="1">
-        <f t="shared" ref="I44" si="12">$F44*H44</f>
-        <v>0.11</v>
-      </c>
-      <c r="J44" s="1">
-        <v>0.11</v>
-      </c>
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="12"/>
       <c r="K44" s="5">
-        <f t="shared" ref="K44" si="13">$F44*J44*50</f>
-        <v>5.5</v>
-      </c>
-      <c r="L44" s="4">
-        <v>3.7999999999999999E-2</v>
-      </c>
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="12"/>
       <c r="M44" s="1">
-        <f t="shared" ref="M44" si="14">$F44*L44*100</f>
-        <v>3.8</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E45" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F45" s="7">
         <v>1</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H45" s="1">
         <v>0.11</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>0.11</v>
       </c>
       <c r="J45" s="1">
         <v>0.11</v>
       </c>
       <c r="K45" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>5.5</v>
       </c>
       <c r="L45" s="4">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="M45" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>3.8</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F46" s="7">
         <v>1</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H46" s="1">
         <v>0.11</v>
       </c>
       <c r="I46" s="1">
-        <f t="shared" ref="I46" si="15">$F46*H46</f>
+        <f t="shared" si="18"/>
         <v>0.11</v>
       </c>
       <c r="J46" s="1">
         <v>0.11</v>
       </c>
       <c r="K46" s="5">
-        <f t="shared" ref="K46" si="16">$F46*J46*50</f>
+        <f t="shared" si="19"/>
         <v>5.5</v>
       </c>
       <c r="L46" s="4">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="M46" s="1">
-        <f t="shared" ref="M46" si="17">$F46*L46*100</f>
+        <f t="shared" si="20"/>
         <v>3.8</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>77</v>
+        <v>67</v>
+      </c>
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="E47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F47" s="7">
         <v>1</v>
       </c>
+      <c r="G47" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0.11</v>
+      </c>
       <c r="I47" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>0.11</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0.11</v>
       </c>
       <c r="K47" s="5">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>5.5</v>
+      </c>
+      <c r="L47" s="4">
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>3.8</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D48" s="7"/>
+        <v>114</v>
+      </c>
+      <c r="C48" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" t="s">
+        <v>97</v>
+      </c>
       <c r="F48" s="7">
         <v>1</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H48" s="1">
-        <v>2.86</v>
+        <v>0.11</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="9"/>
-        <v>2.86</v>
-      </c>
-      <c r="J48" s="5">
-        <v>2.59</v>
+        <f t="shared" si="18"/>
+        <v>0.11</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0.11</v>
       </c>
       <c r="K48" s="5">
-        <f t="shared" si="10"/>
-        <v>129.5</v>
-      </c>
-      <c r="L48" s="1">
-        <v>2.4700000000000002</v>
+        <f t="shared" si="19"/>
+        <v>5.5</v>
+      </c>
+      <c r="L48" s="4">
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M48" s="1">
-        <f t="shared" si="11"/>
-        <v>247.00000000000003</v>
+        <f t="shared" si="20"/>
+        <v>3.8</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="B49" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" t="s">
+        <v>95</v>
       </c>
       <c r="F49" s="7">
         <v>1</v>
       </c>
-      <c r="G49" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="5">
-        <v>3.51</v>
+      <c r="G49" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0.56000000000000005</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="9"/>
-        <v>3.51</v>
-      </c>
-      <c r="J49" s="5">
-        <v>3.21</v>
+        <f t="shared" si="18"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J49" s="4">
+        <v>0.44800000000000001</v>
       </c>
       <c r="K49" s="5">
-        <f t="shared" si="10"/>
-        <v>160.5</v>
-      </c>
-      <c r="L49" s="5">
-        <v>3.02</v>
+        <f t="shared" si="19"/>
+        <v>22.400000000000002</v>
+      </c>
+      <c r="L49" s="4">
+        <v>0.40799999999999997</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" si="11"/>
-        <v>302</v>
+        <f t="shared" si="20"/>
+        <v>40.799999999999997</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="F50" s="7">
         <v>1</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="H50" s="5">
-        <v>39</v>
+        <v>3.51</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="9"/>
-        <v>39</v>
+        <f t="shared" si="18"/>
+        <v>3.51</v>
       </c>
       <c r="J50" s="5">
-        <v>39</v>
+        <v>3.21</v>
       </c>
       <c r="K50" s="5">
-        <f t="shared" si="10"/>
-        <v>1950</v>
+        <f t="shared" si="19"/>
+        <v>160.5</v>
       </c>
       <c r="L50" s="5">
-        <v>39</v>
+        <v>3.02</v>
       </c>
       <c r="M50" s="1">
-        <f t="shared" si="11"/>
-        <v>3900</v>
+        <f t="shared" si="20"/>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="F51" s="7">
         <v>1</v>
       </c>
-      <c r="G51" s="8" t="s">
-        <v>20</v>
+      <c r="G51" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="H51" s="5">
-        <v>0.71</v>
+        <v>39</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="9"/>
-        <v>0.71</v>
+        <f t="shared" si="18"/>
+        <v>39</v>
       </c>
       <c r="J51" s="5">
-        <v>3.21</v>
+        <v>39</v>
       </c>
       <c r="K51" s="5">
-        <f t="shared" si="10"/>
-        <v>160.5</v>
+        <f t="shared" si="19"/>
+        <v>1950</v>
       </c>
       <c r="L51" s="5">
-        <v>0.51619999999999999</v>
+        <v>39</v>
       </c>
       <c r="M51" s="1">
-        <f t="shared" si="11"/>
-        <v>51.62</v>
+        <f t="shared" si="20"/>
+        <v>3900</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F52" s="7">
         <v>1</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H52" s="5">
-        <v>0.76</v>
+        <v>0.71</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="9"/>
-        <v>0.76</v>
+        <f t="shared" si="18"/>
+        <v>0.71</v>
       </c>
       <c r="J52" s="5">
-        <v>0.66300000000000003</v>
+        <v>3.21</v>
       </c>
       <c r="K52" s="5">
-        <f t="shared" si="10"/>
-        <v>33.15</v>
+        <f t="shared" si="19"/>
+        <v>160.5</v>
       </c>
       <c r="L52" s="5">
-        <v>0.56000000000000005</v>
+        <v>0.51619999999999999</v>
       </c>
       <c r="M52" s="1">
-        <f t="shared" si="11"/>
-        <v>56.000000000000007</v>
+        <f t="shared" si="20"/>
+        <v>51.62</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B53" t="s">
-        <v>115</v>
+        <v>13</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="F53" s="7">
         <v>1</v>
       </c>
-      <c r="G53" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H53" s="1">
-        <v>8.1199999999999992</v>
+      <c r="G53" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" s="5">
+        <v>0.76</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" si="9"/>
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="J53" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="K53" s="1">
-        <f t="shared" si="10"/>
-        <v>375</v>
-      </c>
-      <c r="L53" s="1">
-        <v>6.9</v>
+        <f t="shared" si="18"/>
+        <v>0.76</v>
+      </c>
+      <c r="J53" s="5">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="K53" s="5">
+        <f t="shared" si="19"/>
+        <v>33.15</v>
+      </c>
+      <c r="L53" s="5">
+        <v>0.56000000000000005</v>
       </c>
       <c r="M53" s="1">
-        <f t="shared" si="11"/>
-        <v>690</v>
+        <f t="shared" si="20"/>
+        <v>56.000000000000007</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
         <v>109</v>
       </c>
-      <c r="B54" s="13">
+      <c r="C54" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F54" s="7">
+        <v>1</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" s="1">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="I54" s="1">
+        <f t="shared" si="18"/>
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="J54" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="K54" s="1">
+        <f t="shared" si="19"/>
+        <v>375</v>
+      </c>
+      <c r="L54" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="M54" s="1">
+        <f t="shared" si="20"/>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" s="13">
         <v>132193</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F54" s="7">
-        <v>1</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H54" s="1">
+      <c r="C55" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="F55" s="7">
+        <v>1</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="H55" s="1">
         <v>6.12</v>
       </c>
-      <c r="I54" s="1">
-        <f t="shared" si="9"/>
+      <c r="I55" s="1">
+        <f t="shared" si="18"/>
         <v>6.12</v>
       </c>
-      <c r="J54" s="1">
+      <c r="J55" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="K54" s="1">
-        <f t="shared" si="10"/>
+      <c r="K55" s="1">
+        <f t="shared" si="19"/>
         <v>254.99999999999997</v>
       </c>
-      <c r="L54" s="1">
+      <c r="L55" s="1">
         <v>4.8499999999999996</v>
       </c>
-      <c r="M54" s="1">
-        <f t="shared" si="11"/>
+      <c r="M55" s="1">
+        <f t="shared" si="20"/>
         <v>484.99999999999994</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G56" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I56" s="1">
-        <f>SUM(I2:I54)</f>
-        <v>75.95</v>
-      </c>
-      <c r="K56" s="1">
-        <f>SUM(K2:K54)</f>
-        <v>3626.76</v>
-      </c>
-      <c r="M56" s="1">
-        <f>SUM(M2:M54)</f>
-        <v>6777.97</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G57" s="9" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="I57" s="1">
-        <f>I56/1</f>
-        <v>75.95</v>
+        <f>SUM(I2:I55)</f>
+        <v>76.620099999999994</v>
       </c>
       <c r="K57" s="1">
-        <f>K56/50</f>
-        <v>72.535200000000003</v>
+        <f>SUM(K2:K55)</f>
+        <v>3632.69</v>
       </c>
       <c r="M57" s="1">
-        <f>M56/100</f>
-        <v>67.779700000000005</v>
+        <f>SUM(M2:M55)</f>
+        <v>6780.15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G58" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I58" s="1">
+        <f>I57/1</f>
+        <v>76.620099999999994</v>
+      </c>
+      <c r="K58" s="1">
+        <f>K57/50</f>
+        <v>72.653800000000004</v>
+      </c>
+      <c r="M58" s="1">
+        <f>M57/100</f>
+        <v>67.80149999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move several components and traces around
All components except SWD have been connected. May want to route SWD and
button signals on opposite sides.
</commit_message>
<xml_diff>
--- a/specs/base-bom.xlsx
+++ b/specs/base-bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey Zheng\Dropbox\HA-HA\specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzheng13\Documents\HA-HA\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="148">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -462,6 +462,12 @@
   </si>
   <si>
     <t>SMT0403</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>10118194-0001LF</t>
   </si>
 </sst>
 </file>
@@ -828,7 +834,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2115,18 +2121,39 @@
       <c r="A35" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="7"/>
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="7">
+        <v>1</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.46</v>
+      </c>
       <c r="I35" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>0.46</v>
+      </c>
+      <c r="J35" s="4">
+        <v>0.318</v>
       </c>
       <c r="K35" s="5">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>15.9</v>
+      </c>
+      <c r="L35" s="4">
+        <v>0.27500000000000002</v>
       </c>
       <c r="M35" s="1">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>27.500000000000004</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2369,115 +2396,109 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D43" t="s">
-        <v>82</v>
+        <v>141</v>
+      </c>
+      <c r="C43" t="s">
+        <v>135</v>
       </c>
       <c r="F43" s="7">
         <v>1</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H43" s="1">
-        <v>0.46</v>
+        <v>142</v>
+      </c>
+      <c r="H43" s="12">
+        <v>0.34670000000000001</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" ref="I43:I55" si="18">$F43*H43</f>
-        <v>0.46</v>
-      </c>
-      <c r="J43" s="5">
-        <v>0.32900000000000001</v>
+        <f t="shared" ref="I43" si="18">$F43*H43</f>
+        <v>0.34670000000000001</v>
+      </c>
+      <c r="J43" s="12">
+        <v>0.2442</v>
       </c>
       <c r="K43" s="5">
-        <f t="shared" ref="K43:K55" si="19">$F43*J43*50</f>
-        <v>16.45</v>
-      </c>
-      <c r="L43" s="1">
-        <v>0.151</v>
+        <f t="shared" ref="K43" si="19">$F43*J43*50</f>
+        <v>12.21</v>
+      </c>
+      <c r="L43" s="12">
+        <v>0.2442</v>
       </c>
       <c r="M43" s="1">
-        <f t="shared" ref="M43:M55" si="20">$F43*L43*100</f>
-        <v>15.1</v>
+        <f t="shared" ref="M43" si="20">$F43*L43*100</f>
+        <v>24.42</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="7">
+        <v>1</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.46</v>
+      </c>
       <c r="I44" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="J44" s="12"/>
+        <f t="shared" ref="I44:I56" si="21">$F44*H44</f>
+        <v>0.46</v>
+      </c>
+      <c r="J44" s="5">
+        <v>0.32900000000000001</v>
+      </c>
       <c r="K44" s="5">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L44" s="12"/>
+        <f t="shared" ref="K44:K56" si="22">$F44*J44*50</f>
+        <v>16.45</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0.151</v>
+      </c>
       <c r="M44" s="1">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <f t="shared" ref="M44:M56" si="23">$F44*L44*100</f>
+        <v>15.1</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" t="s">
-        <v>114</v>
-      </c>
-      <c r="C45" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E45" t="s">
-        <v>97</v>
-      </c>
-      <c r="F45" s="7">
-        <v>1</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H45" s="1">
-        <v>0.11</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F45" s="7"/>
       <c r="I45" s="1">
-        <f t="shared" si="18"/>
-        <v>0.11</v>
-      </c>
-      <c r="J45" s="1">
-        <v>0.11</v>
-      </c>
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="12"/>
       <c r="K45" s="5">
-        <f t="shared" si="19"/>
-        <v>5.5</v>
-      </c>
-      <c r="L45" s="4">
-        <v>3.7999999999999999E-2</v>
-      </c>
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="L45" s="12"/>
       <c r="M45" s="1">
-        <f t="shared" si="20"/>
-        <v>3.8</v>
+        <f t="shared" si="23"/>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
         <v>108</v>
@@ -2486,7 +2507,7 @@
         <v>79</v>
       </c>
       <c r="E46" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F46" s="7">
         <v>1</v>
@@ -2498,30 +2519,30 @@
         <v>0.11</v>
       </c>
       <c r="I46" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0.11</v>
       </c>
       <c r="J46" s="1">
         <v>0.11</v>
       </c>
       <c r="K46" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5.5</v>
       </c>
       <c r="L46" s="4">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="M46" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>3.8</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C47" t="s">
         <v>108</v>
@@ -2530,7 +2551,7 @@
         <v>79</v>
       </c>
       <c r="E47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F47" s="7">
         <v>1</v>
@@ -2542,30 +2563,30 @@
         <v>0.11</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0.11</v>
       </c>
       <c r="J47" s="1">
         <v>0.11</v>
       </c>
       <c r="K47" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5.5</v>
       </c>
       <c r="L47" s="4">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>3.8</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C48" t="s">
         <v>108</v>
@@ -2574,7 +2595,7 @@
         <v>79</v>
       </c>
       <c r="E48" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F48" s="7">
         <v>1</v>
@@ -2586,36 +2607,39 @@
         <v>0.11</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0.11</v>
       </c>
       <c r="J48" s="1">
         <v>0.11</v>
       </c>
       <c r="K48" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5.5</v>
       </c>
       <c r="L48" s="4">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="M48" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>3.8</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B49" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
-        <v>119</v>
+        <v>108</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="E49" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F49" s="7">
         <v>1</v>
@@ -2624,307 +2648,348 @@
         <v>24</v>
       </c>
       <c r="H49" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.11</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="18"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="J49" s="4">
-        <v>0.44800000000000001</v>
+        <f t="shared" si="21"/>
+        <v>0.11</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0.11</v>
       </c>
       <c r="K49" s="5">
-        <f t="shared" si="19"/>
-        <v>22.400000000000002</v>
+        <f t="shared" si="22"/>
+        <v>5.5</v>
       </c>
       <c r="L49" s="4">
-        <v>0.40799999999999997</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" si="20"/>
-        <v>40.799999999999997</v>
+        <f t="shared" si="23"/>
+        <v>3.8</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
+      </c>
+      <c r="B50" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" t="s">
+        <v>95</v>
       </c>
       <c r="F50" s="7">
         <v>1</v>
       </c>
-      <c r="G50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="5">
-        <v>3.51</v>
+      <c r="G50" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0.56000000000000005</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="18"/>
-        <v>3.51</v>
-      </c>
-      <c r="J50" s="5">
-        <v>3.21</v>
+        <f t="shared" si="21"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J50" s="4">
+        <v>0.44800000000000001</v>
       </c>
       <c r="K50" s="5">
-        <f t="shared" si="19"/>
-        <v>160.5</v>
-      </c>
-      <c r="L50" s="5">
-        <v>3.02</v>
+        <f t="shared" si="22"/>
+        <v>22.400000000000002</v>
+      </c>
+      <c r="L50" s="4">
+        <v>0.40799999999999997</v>
       </c>
       <c r="M50" s="1">
-        <f t="shared" si="20"/>
-        <v>302</v>
+        <f t="shared" si="23"/>
+        <v>40.799999999999997</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="F51" s="7">
         <v>1</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="H51" s="5">
-        <v>39</v>
+        <v>3.51</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="18"/>
-        <v>39</v>
+        <f t="shared" si="21"/>
+        <v>3.51</v>
       </c>
       <c r="J51" s="5">
-        <v>39</v>
+        <v>3.21</v>
       </c>
       <c r="K51" s="5">
-        <f t="shared" si="19"/>
-        <v>1950</v>
+        <f t="shared" si="22"/>
+        <v>160.5</v>
       </c>
       <c r="L51" s="5">
-        <v>39</v>
+        <v>3.02</v>
       </c>
       <c r="M51" s="1">
-        <f t="shared" si="20"/>
-        <v>3900</v>
+        <f t="shared" si="23"/>
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="F52" s="7">
         <v>1</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H52" s="5">
-        <v>0.71</v>
+        <v>39</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="18"/>
-        <v>0.71</v>
+        <f t="shared" si="21"/>
+        <v>39</v>
       </c>
       <c r="J52" s="5">
-        <v>3.21</v>
+        <v>39</v>
       </c>
       <c r="K52" s="5">
-        <f t="shared" si="19"/>
-        <v>160.5</v>
+        <f t="shared" si="22"/>
+        <v>1950</v>
       </c>
       <c r="L52" s="5">
-        <v>0.51619999999999999</v>
+        <v>39</v>
       </c>
       <c r="M52" s="1">
-        <f t="shared" si="20"/>
-        <v>51.62</v>
+        <f t="shared" si="23"/>
+        <v>3900</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F53" s="7">
         <v>1</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H53" s="5">
-        <v>0.76</v>
+        <v>0.71</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" si="18"/>
-        <v>0.76</v>
+        <f t="shared" si="21"/>
+        <v>0.71</v>
       </c>
       <c r="J53" s="5">
-        <v>0.66300000000000003</v>
+        <v>3.21</v>
       </c>
       <c r="K53" s="5">
-        <f t="shared" si="19"/>
-        <v>33.15</v>
+        <f t="shared" si="22"/>
+        <v>160.5</v>
       </c>
       <c r="L53" s="5">
-        <v>0.56000000000000005</v>
+        <v>0.51619999999999999</v>
       </c>
       <c r="M53" s="1">
-        <f t="shared" si="20"/>
-        <v>56.000000000000007</v>
+        <f t="shared" si="23"/>
+        <v>51.62</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B54" t="s">
-        <v>109</v>
+        <v>13</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D54" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E54" s="7" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F54" s="7">
         <v>1</v>
       </c>
-      <c r="G54" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H54" s="1">
-        <v>8.1199999999999992</v>
+      <c r="G54" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H54" s="5">
+        <v>0.76</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" si="18"/>
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="J54" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="K54" s="1">
-        <f t="shared" si="19"/>
-        <v>375</v>
-      </c>
-      <c r="L54" s="1">
-        <v>6.9</v>
+        <f t="shared" si="21"/>
+        <v>0.76</v>
+      </c>
+      <c r="J54" s="5">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="K54" s="5">
+        <f t="shared" si="22"/>
+        <v>33.15</v>
+      </c>
+      <c r="L54" s="5">
+        <v>0.56000000000000005</v>
       </c>
       <c r="M54" s="1">
-        <f t="shared" si="20"/>
-        <v>690</v>
+        <f t="shared" si="23"/>
+        <v>56.000000000000007</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55" s="7">
+        <v>1</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H55" s="1">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="I55" s="1">
+        <f t="shared" si="21"/>
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="J55" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="K55" s="1">
+        <f t="shared" si="22"/>
+        <v>375</v>
+      </c>
+      <c r="L55" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="M55" s="1">
+        <f t="shared" si="23"/>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B55" s="13">
+      <c r="B56" s="13">
         <v>132193</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D55" s="7"/>
-      <c r="F55" s="7">
-        <v>1</v>
-      </c>
-      <c r="G55" s="9" t="s">
+      <c r="D56" s="7"/>
+      <c r="F56" s="7">
+        <v>1</v>
+      </c>
+      <c r="G56" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="H55" s="1">
+      <c r="H56" s="1">
         <v>6.12</v>
       </c>
-      <c r="I55" s="1">
-        <f t="shared" si="18"/>
+      <c r="I56" s="1">
+        <f t="shared" si="21"/>
         <v>6.12</v>
       </c>
-      <c r="J55" s="1">
+      <c r="J56" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="K55" s="1">
-        <f t="shared" si="19"/>
+      <c r="K56" s="1">
+        <f t="shared" si="22"/>
         <v>254.99999999999997</v>
       </c>
-      <c r="L55" s="1">
+      <c r="L56" s="1">
         <v>4.8499999999999996</v>
       </c>
-      <c r="M55" s="1">
-        <f t="shared" si="20"/>
+      <c r="M56" s="1">
+        <f t="shared" si="23"/>
         <v>484.99999999999994</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G57" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I57" s="1">
-        <f>SUM(I2:I55)</f>
-        <v>76.620099999999994</v>
-      </c>
-      <c r="K57" s="1">
-        <f>SUM(K2:K55)</f>
-        <v>3632.69</v>
-      </c>
-      <c r="M57" s="1">
-        <f>SUM(M2:M55)</f>
-        <v>6780.15</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G58" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I58" s="1">
+        <f>SUM(I2:I56)</f>
+        <v>77.4268</v>
+      </c>
+      <c r="K58" s="1">
+        <f>SUM(K2:K56)</f>
+        <v>3660.8</v>
+      </c>
+      <c r="M58" s="1">
+        <f>SUM(M2:M56)</f>
+        <v>6832.07</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G59" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="I58" s="1">
-        <f>I57/1</f>
-        <v>76.620099999999994</v>
-      </c>
-      <c r="K58" s="1">
-        <f>K57/50</f>
-        <v>72.653800000000004</v>
-      </c>
-      <c r="M58" s="1">
-        <f>M57/100</f>
-        <v>67.80149999999999</v>
+      <c r="I59" s="1">
+        <f>I58/1</f>
+        <v>77.4268</v>
+      </c>
+      <c r="K59" s="1">
+        <f>K58/50</f>
+        <v>73.216000000000008</v>
+      </c>
+      <c r="M59" s="1">
+        <f>M58/100</f>
+        <v>68.320700000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new dimensions for base station
</commit_message>
<xml_diff>
--- a/specs/base-bom.xlsx
+++ b/specs/base-bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzheng13\Documents\HA-HA\specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey Zheng\Dropbox\HA-HA\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -440,9 +440,6 @@
     <t>Preci-Dip</t>
   </si>
   <si>
-    <t>3309W-1-103</t>
-  </si>
-  <si>
     <t>OSTTE020104</t>
   </si>
   <si>
@@ -468,6 +465,9 @@
   </si>
   <si>
     <t>10118194-0001LF</t>
+  </si>
+  <si>
+    <t>3319W-1-103</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1221,7 @@
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
         <v>106</v>
@@ -1230,7 +1230,7 @@
         <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F14" s="7">
         <v>1</v>
@@ -1265,16 +1265,16 @@
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
         <v>106</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F15" s="7">
         <v>1</v>
@@ -2122,7 +2122,7 @@
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C35" t="s">
         <v>112</v>
@@ -2285,7 +2285,7 @@
         <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
         <v>135</v>
@@ -2294,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H40" s="12">
         <v>0.34670000000000001</v>
@@ -2323,7 +2323,7 @@
         <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C41" t="s">
         <v>135</v>
@@ -2332,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H41" s="12">
         <v>0.34670000000000001</v>
@@ -2361,7 +2361,7 @@
         <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C42" t="s">
         <v>135</v>
@@ -2370,7 +2370,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H42" s="12">
         <v>0.34670000000000001</v>
@@ -2396,10 +2396,10 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B43" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C43" t="s">
         <v>135</v>
@@ -2408,7 +2408,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H43" s="12">
         <v>0.34670000000000001</v>
@@ -2674,7 +2674,7 @@
         <v>73</v>
       </c>
       <c r="B50" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C50" t="s">
         <v>119</v>
@@ -2689,25 +2689,25 @@
         <v>24</v>
       </c>
       <c r="H50" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.4</v>
       </c>
       <c r="I50" s="1">
         <f t="shared" si="21"/>
-        <v>0.56000000000000005</v>
+        <v>0.4</v>
       </c>
       <c r="J50" s="4">
-        <v>0.44800000000000001</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="K50" s="5">
         <f t="shared" si="22"/>
-        <v>22.400000000000002</v>
+        <v>15.950000000000001</v>
       </c>
       <c r="L50" s="4">
-        <v>0.40799999999999997</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="M50" s="1">
         <f t="shared" si="23"/>
-        <v>40.799999999999997</v>
+        <v>28.599999999999998</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -2964,15 +2964,15 @@
       </c>
       <c r="I58" s="1">
         <f>SUM(I2:I56)</f>
-        <v>77.4268</v>
+        <v>77.266800000000003</v>
       </c>
       <c r="K58" s="1">
         <f>SUM(K2:K56)</f>
-        <v>3660.8</v>
+        <v>3654.3500000000004</v>
       </c>
       <c r="M58" s="1">
         <f>SUM(M2:M56)</f>
-        <v>6832.07</v>
+        <v>6819.87</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -2981,15 +2981,15 @@
       </c>
       <c r="I59" s="1">
         <f>I58/1</f>
-        <v>77.4268</v>
+        <v>77.266800000000003</v>
       </c>
       <c r="K59" s="1">
         <f>K58/50</f>
-        <v>73.216000000000008</v>
+        <v>73.087000000000003</v>
       </c>
       <c r="M59" s="1">
         <f>M58/100</f>
-        <v>68.320700000000002</v>
+        <v>68.198700000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix base station dimensions and cleanup datasheets
</commit_message>
<xml_diff>
--- a/specs/base-bom.xlsx
+++ b/specs/base-bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey Zheng\Dropbox\HA-HA\specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzheng13\Documents\HA-HA\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="138">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -149,36 +149,12 @@
     <t>FB1</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
     <t>R3</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
     <t>C8</t>
   </si>
   <si>
@@ -231,12 +207,6 @@
   </si>
   <si>
     <t>R5</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>L2</t>
   </si>
   <si>
     <t>L3</t>
@@ -834,7 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M59"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -865,10 +838,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
@@ -916,21 +889,21 @@
         <v>0.52</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I32" si="0">$F2*H2</f>
+        <f t="shared" ref="I2:I25" si="0">$F2*H2</f>
         <v>0.52</v>
       </c>
       <c r="J2" s="5">
         <v>0.44700000000000001</v>
       </c>
       <c r="K2" s="5">
-        <f t="shared" ref="K2:K32" si="1">$F2*J2*50</f>
+        <f t="shared" ref="K2:K25" si="1">$F2*J2*50</f>
         <v>22.35</v>
       </c>
       <c r="L2" s="1">
         <v>0.435</v>
       </c>
       <c r="M2" s="1">
-        <f t="shared" ref="M2:M32" si="2">$F2*L2*100</f>
+        <f t="shared" ref="M2:M25" si="2">$F2*L2*100</f>
         <v>43.5</v>
       </c>
     </row>
@@ -1092,146 +1065,328 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="J7" s="4">
+        <v>2.3E-2</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1.6E-2</v>
       </c>
       <c r="M7" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="I8" si="3">$F8*H8</f>
+        <v>0.1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2.3E-2</v>
       </c>
       <c r="K8" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="K8" si="4">$F8*J8*50</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1.6E-2</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="M8" si="5">$F8*L8*100</f>
+        <v>1.6</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K9" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.65</v>
+      </c>
+      <c r="L9" s="4">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1.4E-2</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="L10" s="4">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M10" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="I11:I12" si="6">$F11*H11</f>
+        <v>0.1</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1.4E-2</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="K11:K12" si="7">$F11*J11*50</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="L11" s="4">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="M11:M12" si="8">$F11*L11*100</f>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1.4E-2</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="L12" s="4">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="7"/>
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.13</v>
+      </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.13</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.115</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.75</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.104</v>
       </c>
       <c r="M13" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
         <v>79</v>
       </c>
-      <c r="E14" t="s">
-        <v>142</v>
-      </c>
       <c r="F14" s="7">
         <v>1</v>
       </c>
@@ -1242,39 +1397,39 @@
         <v>0.1</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I14" si="9">$F14*H14</f>
         <v>0.1</v>
       </c>
       <c r="J14" s="4">
-        <v>2.3E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K14" s="5">
-        <f t="shared" si="1"/>
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L14" s="4">
-        <v>1.6E-2</v>
+        <f t="shared" ref="K14" si="10">$F14*J14*50</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="L14" s="12">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6</v>
+        <f t="shared" ref="M14" si="11">$F14*L14*100</f>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="F15" s="7">
         <v>1</v>
@@ -1286,39 +1441,39 @@
         <v>0.1</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" ref="I15" si="3">$F15*H15</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="J15" s="4">
-        <v>2.3E-2</v>
+        <v>0.06</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" ref="K15" si="4">$F15*J15*50</f>
-        <v>1.1499999999999999</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="L15" s="4">
-        <v>1.6E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" ref="M15" si="5">$F15*L15*100</f>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>2.7</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F16" s="7">
         <v>1</v>
@@ -1334,55 +1489,55 @@
         <v>0.1</v>
       </c>
       <c r="J16" s="4">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" si="1"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="L16" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="4">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K17" s="10">
         <f t="shared" si="1"/>
         <v>0.65</v>
-      </c>
-      <c r="L16" s="4">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="M16" s="1">
-        <f t="shared" si="2"/>
-        <v>0.89999999999999991</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" t="s">
-        <v>120</v>
-      </c>
-      <c r="C17" t="s">
-        <v>106</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="7">
-        <v>1</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="I17" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="J17" s="4">
-        <v>1.4E-2</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" si="1"/>
-        <v>0.70000000000000007</v>
       </c>
       <c r="L17" s="4">
         <v>8.9999999999999993E-3</v>
@@ -1394,19 +1549,19 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
@@ -1418,39 +1573,39 @@
         <v>0.1</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" ref="I18:I19" si="6">$F18*H18</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="J18" s="4">
-        <v>1.4E-2</v>
-      </c>
-      <c r="K18" s="5">
-        <f t="shared" ref="K18:K19" si="7">$F18*J18*50</f>
-        <v>0.70000000000000007</v>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K18" s="10">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
       </c>
       <c r="L18" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" ref="M18:M19" si="8">$F18*L18*100</f>
+        <f t="shared" si="2"/>
         <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F19" s="7">
         <v>1</v>
@@ -1462,39 +1617,39 @@
         <v>0.1</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="J19" s="4">
-        <v>1.4E-2</v>
-      </c>
-      <c r="K19" s="5">
-        <f t="shared" si="7"/>
-        <v>0.70000000000000007</v>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K19" s="10">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
       </c>
       <c r="L19" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="F20" s="7">
         <v>1</v>
@@ -1503,42 +1658,42 @@
         <v>24</v>
       </c>
       <c r="H20" s="1">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="0"/>
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="J20" s="4">
-        <v>0.115</v>
+        <v>2.3E-2</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>5.75</v>
-      </c>
-      <c r="L20" s="1">
-        <v>0.104</v>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L20" s="4">
+        <v>1.6E-2</v>
       </c>
       <c r="M20" s="1">
         <f t="shared" si="2"/>
-        <v>10.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F21" s="7">
         <v>1</v>
@@ -1550,39 +1705,39 @@
         <v>0.1</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" ref="I21" si="9">$F21*H21</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="J21" s="4">
-        <v>1.4E-2</v>
-      </c>
-      <c r="K21" s="5">
-        <f t="shared" ref="K21" si="10">$F21*J21*50</f>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="L21" s="12">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K21" s="10">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
+      <c r="L21" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" ref="M21" si="11">$F21*L21*100</f>
+        <f t="shared" si="2"/>
         <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F22" s="7">
         <v>1</v>
@@ -1591,174 +1746,157 @@
         <v>24</v>
       </c>
       <c r="H22" s="1">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="J22" s="4">
-        <v>0.06</v>
+        <v>6.2E-2</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="L22" s="4">
-        <v>2.7E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="M22" s="1">
         <f t="shared" si="2"/>
-        <v>2.7</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" t="s">
-        <v>90</v>
+        <v>119</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="F23" s="7">
         <v>1</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0.1</v>
+      <c r="G23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="5">
+        <v>9.48</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="J23" s="4">
-        <v>8.9999999999999993E-3</v>
+        <v>9.48</v>
+      </c>
+      <c r="J23" s="5">
+        <v>7.65</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="L23" s="4">
-        <v>6.0000000000000001E-3</v>
+        <v>382.5</v>
+      </c>
+      <c r="L23" s="5">
+        <v>7.53</v>
       </c>
       <c r="M23" s="1">
         <f t="shared" si="2"/>
-        <v>0.6</v>
+        <v>753</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="F24" s="7">
         <v>1</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H24" s="1">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J24" s="4">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="K24" s="10">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="K24" s="5">
         <f t="shared" si="1"/>
-        <v>0.65</v>
-      </c>
-      <c r="L24" s="4">
-        <v>8.9999999999999993E-3</v>
+        <v>13.600000000000001</v>
+      </c>
+      <c r="L24" s="12">
+        <v>0.22389999999999999</v>
       </c>
       <c r="M24" s="1">
         <f t="shared" si="2"/>
-        <v>0.89999999999999991</v>
+        <v>22.39</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>62</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="F25" s="7">
         <v>1</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H25" s="1">
-        <v>0.1</v>
+        <v>0.91</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.91</v>
       </c>
       <c r="J25" s="4">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="K25" s="10">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="K25" s="5">
         <f t="shared" si="1"/>
-        <v>0.65</v>
-      </c>
-      <c r="L25" s="4">
-        <v>8.9999999999999993E-3</v>
+        <v>39.800000000000004</v>
+      </c>
+      <c r="L25" s="12">
+        <v>0.68659999999999999</v>
       </c>
       <c r="M25" s="1">
         <f t="shared" si="2"/>
-        <v>0.89999999999999991</v>
+        <v>68.66</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F26" s="7">
         <v>1</v>
@@ -1770,84 +1908,73 @@
         <v>0.1</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="J26" s="4">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="K26" s="10">
-        <f t="shared" si="1"/>
-        <v>0.65</v>
-      </c>
-      <c r="L26" s="4">
-        <v>8.9999999999999993E-3</v>
+        <f t="shared" ref="I26:I31" si="12">$F26*H26</f>
+        <v>0.1</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" ref="K26:K31" si="13">$F26*J26*50</f>
+        <v>2.5</v>
+      </c>
+      <c r="L26" s="1">
+        <v>4.3299999999999998E-2</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="2"/>
-        <v>0.89999999999999991</v>
+        <f t="shared" ref="M26:M31" si="14">$F26*L26*100</f>
+        <v>4.33</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="F27" s="7">
         <v>1</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H27" s="1">
-        <v>0.1</v>
+        <v>0.62</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="J27" s="4">
-        <v>2.3E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.62</v>
+      </c>
+      <c r="J27" s="12">
+        <v>0.4632</v>
       </c>
       <c r="K27" s="5">
-        <f t="shared" si="1"/>
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L27" s="4">
-        <v>1.6E-2</v>
+        <f t="shared" si="13"/>
+        <v>23.16</v>
+      </c>
+      <c r="L27" s="12">
+        <v>0.44390000000000002</v>
       </c>
       <c r="M27" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6</v>
+        <f t="shared" si="14"/>
+        <v>44.39</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" t="s">
-        <v>88</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E28" s="11"/>
       <c r="F28" s="7">
         <v>1</v>
       </c>
@@ -1855,42 +1982,42 @@
         <v>24</v>
       </c>
       <c r="H28" s="1">
-        <v>0.1</v>
+        <v>0.46</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
+        <f t="shared" si="12"/>
+        <v>0.46</v>
       </c>
       <c r="J28" s="4">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="K28" s="10">
-        <f t="shared" si="1"/>
-        <v>0.65</v>
+        <v>0.318</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" si="13"/>
+        <v>15.9</v>
       </c>
       <c r="L28" s="4">
-        <v>8.9999999999999993E-3</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" si="2"/>
-        <v>0.89999999999999991</v>
+        <f t="shared" si="14"/>
+        <v>27.500000000000004</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F29" s="7">
         <v>1</v>
@@ -1899,235 +2026,236 @@
         <v>24</v>
       </c>
       <c r="H29" s="1">
-        <v>0.16</v>
+        <v>0.1</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
+        <f t="shared" si="12"/>
+        <v>0.1</v>
       </c>
       <c r="J29" s="4">
-        <v>6.2E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="K29" s="5">
-        <f t="shared" si="1"/>
-        <v>3.1</v>
+        <f t="shared" si="13"/>
+        <v>3.55</v>
       </c>
       <c r="L29" s="4">
-        <v>4.2999999999999997E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="M29" s="1">
-        <f t="shared" si="2"/>
-        <v>4.3</v>
+        <f t="shared" si="14"/>
+        <v>6.1</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7" t="s">
-        <v>130</v>
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" t="s">
+        <v>84</v>
       </c>
       <c r="F30" s="7">
         <v>1</v>
       </c>
-      <c r="G30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="5">
-        <v>9.48</v>
+      <c r="G30" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.1</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="0"/>
-        <v>9.48</v>
-      </c>
-      <c r="J30" s="5">
-        <v>7.65</v>
+        <f t="shared" si="12"/>
+        <v>0.1</v>
+      </c>
+      <c r="J30" s="4">
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="K30" s="5">
-        <f t="shared" si="1"/>
-        <v>382.5</v>
-      </c>
-      <c r="L30" s="5">
-        <v>7.53</v>
+        <f t="shared" si="13"/>
+        <v>2.4</v>
+      </c>
+      <c r="L30" s="4">
+        <v>3.9E-2</v>
       </c>
       <c r="M30" s="1">
-        <f t="shared" si="2"/>
-        <v>753</v>
+        <f t="shared" si="14"/>
+        <v>3.9</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" t="s">
+        <v>125</v>
+      </c>
+      <c r="F31" s="7">
+        <v>1</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31" s="7">
-        <v>1</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="1">
-        <v>0.3</v>
+      <c r="H31" s="12">
+        <v>0.34670000000000001</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="J31" s="4">
-        <v>0.27200000000000002</v>
+        <f t="shared" si="12"/>
+        <v>0.34670000000000001</v>
+      </c>
+      <c r="J31" s="12">
+        <v>0.2442</v>
       </c>
       <c r="K31" s="5">
-        <f t="shared" si="1"/>
-        <v>13.600000000000001</v>
+        <f t="shared" si="13"/>
+        <v>12.21</v>
       </c>
       <c r="L31" s="12">
-        <v>0.22389999999999999</v>
+        <v>0.2442</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" si="2"/>
-        <v>22.39</v>
+        <f t="shared" si="14"/>
+        <v>24.42</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>128</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="F32" s="7">
         <v>1</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="1">
-        <v>0.91</v>
+        <v>131</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0.34670000000000001</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="0"/>
-        <v>0.91</v>
-      </c>
-      <c r="J32" s="4">
-        <v>0.79600000000000004</v>
+        <f t="shared" ref="I32:I33" si="15">$F32*H32</f>
+        <v>0.34670000000000001</v>
+      </c>
+      <c r="J32" s="12">
+        <v>0.2442</v>
       </c>
       <c r="K32" s="5">
-        <f t="shared" si="1"/>
-        <v>39.800000000000004</v>
+        <f t="shared" ref="K32:K33" si="16">$F32*J32*50</f>
+        <v>12.21</v>
       </c>
       <c r="L32" s="12">
-        <v>0.68659999999999999</v>
+        <v>0.2442</v>
       </c>
       <c r="M32" s="1">
-        <f t="shared" si="2"/>
-        <v>68.66</v>
+        <f t="shared" ref="M32:M33" si="17">$F32*L32*100</f>
+        <v>24.42</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="F33" s="7">
         <v>1</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H33" s="1">
-        <v>0.1</v>
+        <v>131</v>
+      </c>
+      <c r="H33" s="12">
+        <v>0.34670000000000001</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" ref="I33:I40" si="12">$F33*H33</f>
-        <v>0.1</v>
-      </c>
-      <c r="J33" s="1">
-        <v>0.05</v>
+        <f t="shared" si="15"/>
+        <v>0.34670000000000001</v>
+      </c>
+      <c r="J33" s="12">
+        <v>0.2442</v>
       </c>
       <c r="K33" s="5">
-        <f t="shared" ref="K33:K40" si="13">$F33*J33*50</f>
-        <v>2.5</v>
-      </c>
-      <c r="L33" s="1">
-        <v>4.3299999999999998E-2</v>
+        <f t="shared" si="16"/>
+        <v>12.21</v>
+      </c>
+      <c r="L33" s="12">
+        <v>0.2442</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" ref="M33:M40" si="14">$F33*L33*100</f>
-        <v>4.33</v>
+        <f t="shared" si="17"/>
+        <v>24.42</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C34" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F34" s="7">
         <v>1</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34" s="1">
-        <v>0.62</v>
+        <v>131</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0.34670000000000001</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="12"/>
-        <v>0.62</v>
+        <f t="shared" ref="I34" si="18">$F34*H34</f>
+        <v>0.34670000000000001</v>
       </c>
       <c r="J34" s="12">
-        <v>0.4632</v>
+        <v>0.2442</v>
       </c>
       <c r="K34" s="5">
-        <f t="shared" si="13"/>
-        <v>23.16</v>
+        <f t="shared" ref="K34" si="19">$F34*J34*50</f>
+        <v>12.21</v>
       </c>
       <c r="L34" s="12">
-        <v>0.44390000000000002</v>
+        <v>0.2442</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" si="14"/>
-        <v>44.39</v>
+        <f t="shared" ref="M34" si="20">$F34*L34*100</f>
+        <v>24.42</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
-      </c>
-      <c r="C35" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35" s="11"/>
+        <v>35</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" t="s">
+        <v>72</v>
+      </c>
       <c r="F35" s="7">
         <v>1</v>
       </c>
@@ -2138,75 +2266,127 @@
         <v>0.46</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="I35:I46" si="21">$F35*H35</f>
         <v>0.46</v>
       </c>
-      <c r="J35" s="4">
-        <v>0.318</v>
+      <c r="J35" s="5">
+        <v>0.32900000000000001</v>
       </c>
       <c r="K35" s="5">
-        <f t="shared" si="13"/>
-        <v>15.9</v>
-      </c>
-      <c r="L35" s="4">
-        <v>0.27500000000000002</v>
+        <f t="shared" ref="K35:K46" si="22">$F35*J35*50</f>
+        <v>16.45</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0.151</v>
       </c>
       <c r="M35" s="1">
-        <f t="shared" si="14"/>
-        <v>27.500000000000004</v>
+        <f t="shared" ref="M35:M46" si="23">$F35*L35*100</f>
+        <v>15.1</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="7"/>
+      <c r="E36" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.11</v>
+      </c>
       <c r="I36" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="21"/>
+        <v>0.11</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0.11</v>
       </c>
       <c r="K36" s="5">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>5.5</v>
+      </c>
+      <c r="L36" s="4">
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M36" s="1">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>3.8</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" t="s">
+        <v>86</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.11</v>
+      </c>
       <c r="I37" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="21"/>
+        <v>0.11</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.11</v>
       </c>
       <c r="K37" s="5">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>5.5</v>
+      </c>
+      <c r="L37" s="4">
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M37" s="1">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>3.8</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E38" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
@@ -2215,42 +2395,42 @@
         <v>24</v>
       </c>
       <c r="H38" s="1">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
-      </c>
-      <c r="J38" s="4">
-        <v>7.0999999999999994E-2</v>
+        <f t="shared" si="21"/>
+        <v>0.11</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0.11</v>
       </c>
       <c r="K38" s="5">
-        <f t="shared" si="13"/>
-        <v>3.55</v>
+        <f t="shared" si="22"/>
+        <v>5.5</v>
       </c>
       <c r="L38" s="4">
-        <v>6.0999999999999999E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M38" s="1">
-        <f t="shared" si="14"/>
-        <v>6.1</v>
+        <f t="shared" si="23"/>
+        <v>3.8</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="E39" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F39" s="7">
         <v>1</v>
@@ -2259,736 +2439,347 @@
         <v>24</v>
       </c>
       <c r="H39" s="1">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
-      </c>
-      <c r="J39" s="4">
-        <v>4.8000000000000001E-2</v>
+        <f t="shared" si="21"/>
+        <v>0.11</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0.11</v>
       </c>
       <c r="K39" s="5">
-        <f t="shared" si="13"/>
-        <v>2.4</v>
+        <f t="shared" si="22"/>
+        <v>5.5</v>
       </c>
       <c r="L39" s="4">
-        <v>3.9E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M39" s="1">
-        <f t="shared" si="14"/>
-        <v>3.9</v>
+        <f t="shared" si="23"/>
+        <v>3.8</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
+        <v>109</v>
+      </c>
+      <c r="E40" t="s">
+        <v>85</v>
       </c>
       <c r="F40" s="7">
         <v>1</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="H40" s="12">
-        <v>0.34670000000000001</v>
+        <v>24</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.4</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" si="12"/>
-        <v>0.34670000000000001</v>
-      </c>
-      <c r="J40" s="12">
-        <v>0.2442</v>
+        <f t="shared" si="21"/>
+        <v>0.4</v>
+      </c>
+      <c r="J40" s="4">
+        <v>0.31900000000000001</v>
       </c>
       <c r="K40" s="5">
-        <f t="shared" si="13"/>
-        <v>12.21</v>
-      </c>
-      <c r="L40" s="12">
-        <v>0.2442</v>
+        <f t="shared" si="22"/>
+        <v>15.950000000000001</v>
+      </c>
+      <c r="L40" s="4">
+        <v>0.28599999999999998</v>
       </c>
       <c r="M40" s="1">
-        <f t="shared" si="14"/>
-        <v>24.42</v>
+        <f t="shared" si="23"/>
+        <v>28.599999999999998</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" t="s">
-        <v>139</v>
-      </c>
-      <c r="C41" t="s">
-        <v>135</v>
+        <v>11</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="F41" s="7">
         <v>1</v>
       </c>
-      <c r="G41" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="H41" s="12">
-        <v>0.34670000000000001</v>
+      <c r="G41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="5">
+        <v>3.51</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" ref="I41:I42" si="15">$F41*H41</f>
-        <v>0.34670000000000001</v>
-      </c>
-      <c r="J41" s="12">
-        <v>0.2442</v>
+        <f t="shared" si="21"/>
+        <v>3.51</v>
+      </c>
+      <c r="J41" s="5">
+        <v>3.21</v>
       </c>
       <c r="K41" s="5">
-        <f t="shared" ref="K41:K42" si="16">$F41*J41*50</f>
-        <v>12.21</v>
-      </c>
-      <c r="L41" s="12">
-        <v>0.2442</v>
+        <f t="shared" si="22"/>
+        <v>160.5</v>
+      </c>
+      <c r="L41" s="5">
+        <v>3.02</v>
       </c>
       <c r="M41" s="1">
-        <f t="shared" ref="M41:M42" si="17">$F41*L41*100</f>
-        <v>24.42</v>
+        <f t="shared" si="23"/>
+        <v>302</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" t="s">
-        <v>140</v>
-      </c>
-      <c r="C42" t="s">
-        <v>135</v>
+        <v>14</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="F42" s="7">
         <v>1</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="H42" s="12">
-        <v>0.34670000000000001</v>
+      <c r="G42" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="5">
+        <v>39</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" si="15"/>
-        <v>0.34670000000000001</v>
-      </c>
-      <c r="J42" s="12">
-        <v>0.2442</v>
+        <f t="shared" si="21"/>
+        <v>39</v>
+      </c>
+      <c r="J42" s="5">
+        <v>39</v>
       </c>
       <c r="K42" s="5">
-        <f t="shared" si="16"/>
-        <v>12.21</v>
-      </c>
-      <c r="L42" s="12">
-        <v>0.2442</v>
+        <f t="shared" si="22"/>
+        <v>1950</v>
+      </c>
+      <c r="L42" s="5">
+        <v>39</v>
       </c>
       <c r="M42" s="1">
-        <f t="shared" si="17"/>
-        <v>24.42</v>
+        <f t="shared" si="23"/>
+        <v>3900</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B43" t="s">
-        <v>140</v>
-      </c>
-      <c r="C43" t="s">
-        <v>135</v>
+        <v>12</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="F43" s="7">
         <v>1</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="H43" s="12">
-        <v>0.34670000000000001</v>
+      <c r="G43" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0.71</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" ref="I43" si="18">$F43*H43</f>
-        <v>0.34670000000000001</v>
-      </c>
-      <c r="J43" s="12">
-        <v>0.2442</v>
+        <f t="shared" si="21"/>
+        <v>0.71</v>
+      </c>
+      <c r="J43" s="5">
+        <v>3.21</v>
       </c>
       <c r="K43" s="5">
-        <f t="shared" ref="K43" si="19">$F43*J43*50</f>
-        <v>12.21</v>
-      </c>
-      <c r="L43" s="12">
-        <v>0.2442</v>
+        <f t="shared" si="22"/>
+        <v>160.5</v>
+      </c>
+      <c r="L43" s="5">
+        <v>0.51619999999999999</v>
       </c>
       <c r="M43" s="1">
-        <f t="shared" ref="M43" si="20">$F43*L43*100</f>
-        <v>24.42</v>
+        <f t="shared" si="23"/>
+        <v>51.62</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" t="s">
-        <v>35</v>
+        <v>13</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D44" t="s">
-        <v>82</v>
+        <v>23</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="F44" s="7">
         <v>1</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H44" s="1">
-        <v>0.46</v>
+      <c r="G44" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0.76</v>
       </c>
       <c r="I44" s="1">
-        <f t="shared" ref="I44:I56" si="21">$F44*H44</f>
-        <v>0.46</v>
+        <f t="shared" si="21"/>
+        <v>0.76</v>
       </c>
       <c r="J44" s="5">
-        <v>0.32900000000000001</v>
+        <v>0.66300000000000003</v>
       </c>
       <c r="K44" s="5">
-        <f t="shared" ref="K44:K56" si="22">$F44*J44*50</f>
-        <v>16.45</v>
-      </c>
-      <c r="L44" s="1">
-        <v>0.151</v>
+        <f t="shared" si="22"/>
+        <v>33.15</v>
+      </c>
+      <c r="L44" s="5">
+        <v>0.56000000000000005</v>
       </c>
       <c r="M44" s="1">
-        <f t="shared" ref="M44:M56" si="23">$F44*L44*100</f>
-        <v>15.1</v>
+        <f t="shared" si="23"/>
+        <v>56.000000000000007</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45" s="7"/>
+        <v>94</v>
+      </c>
+      <c r="B45" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" s="1">
+        <v>8.1199999999999992</v>
+      </c>
       <c r="I45" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="J45" s="12"/>
-      <c r="K45" s="5">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="J45" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="K45" s="1">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="L45" s="12"/>
+        <v>375</v>
+      </c>
+      <c r="L45" s="1">
+        <v>6.9</v>
+      </c>
       <c r="M45" s="1">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>690</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" t="s">
-        <v>108</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" t="s">
-        <v>97</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B46" s="13">
+        <v>132193</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="7"/>
       <c r="F46" s="7">
         <v>1</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="H46" s="1">
-        <v>0.11</v>
+        <v>6.12</v>
       </c>
       <c r="I46" s="1">
         <f t="shared" si="21"/>
-        <v>0.11</v>
+        <v>6.12</v>
       </c>
       <c r="J46" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="K46" s="5">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="K46" s="1">
         <f t="shared" si="22"/>
-        <v>5.5</v>
-      </c>
-      <c r="L46" s="4">
-        <v>3.7999999999999999E-2</v>
+        <v>254.99999999999997</v>
+      </c>
+      <c r="L46" s="1">
+        <v>4.8499999999999996</v>
       </c>
       <c r="M46" s="1">
         <f t="shared" si="23"/>
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C47" t="s">
-        <v>108</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" t="s">
-        <v>96</v>
-      </c>
-      <c r="F47" s="7">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H47" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="I47" s="1">
-        <f t="shared" si="21"/>
-        <v>0.11</v>
-      </c>
-      <c r="J47" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="K47" s="5">
-        <f t="shared" si="22"/>
-        <v>5.5</v>
-      </c>
-      <c r="L47" s="4">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="M47" s="1">
-        <f t="shared" si="23"/>
-        <v>3.8</v>
+        <v>484.99999999999994</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" t="s">
-        <v>108</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E48" t="s">
-        <v>98</v>
-      </c>
-      <c r="F48" s="7">
-        <v>1</v>
-      </c>
       <c r="G48" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H48" s="1">
-        <v>0.11</v>
+        <v>5</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="21"/>
-        <v>0.11</v>
-      </c>
-      <c r="J48" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="K48" s="5">
-        <f t="shared" si="22"/>
-        <v>5.5</v>
-      </c>
-      <c r="L48" s="4">
-        <v>3.7999999999999999E-2</v>
+        <f>SUM(I2:I46)</f>
+        <v>77.266800000000003</v>
+      </c>
+      <c r="K48" s="1">
+        <f>SUM(K2:K46)</f>
+        <v>3654.3500000000004</v>
       </c>
       <c r="M48" s="1">
-        <f t="shared" si="23"/>
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B49" t="s">
-        <v>114</v>
-      </c>
-      <c r="C49" t="s">
-        <v>108</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E49" t="s">
-        <v>97</v>
-      </c>
-      <c r="F49" s="7">
-        <v>1</v>
-      </c>
+        <f>SUM(M2:M46)</f>
+        <v>6819.87</v>
+      </c>
+    </row>
+    <row r="49" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G49" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H49" s="1">
-        <v>0.11</v>
+        <v>71</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="21"/>
-        <v>0.11</v>
-      </c>
-      <c r="J49" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="K49" s="5">
-        <f t="shared" si="22"/>
-        <v>5.5</v>
-      </c>
-      <c r="L49" s="4">
-        <v>3.7999999999999999E-2</v>
+        <f>I48/1</f>
+        <v>77.266800000000003</v>
+      </c>
+      <c r="K49" s="1">
+        <f>K48/50</f>
+        <v>73.087000000000003</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" si="23"/>
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50" t="s">
-        <v>147</v>
-      </c>
-      <c r="C50" t="s">
-        <v>119</v>
-      </c>
-      <c r="E50" t="s">
-        <v>95</v>
-      </c>
-      <c r="F50" s="7">
-        <v>1</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H50" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I50" s="1">
-        <f t="shared" si="21"/>
-        <v>0.4</v>
-      </c>
-      <c r="J50" s="4">
-        <v>0.31900000000000001</v>
-      </c>
-      <c r="K50" s="5">
-        <f t="shared" si="22"/>
-        <v>15.950000000000001</v>
-      </c>
-      <c r="L50" s="4">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="M50" s="1">
-        <f t="shared" si="23"/>
-        <v>28.599999999999998</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F51" s="7">
-        <v>1</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H51" s="5">
-        <v>3.51</v>
-      </c>
-      <c r="I51" s="1">
-        <f t="shared" si="21"/>
-        <v>3.51</v>
-      </c>
-      <c r="J51" s="5">
-        <v>3.21</v>
-      </c>
-      <c r="K51" s="5">
-        <f t="shared" si="22"/>
-        <v>160.5</v>
-      </c>
-      <c r="L51" s="5">
-        <v>3.02</v>
-      </c>
-      <c r="M51" s="1">
-        <f t="shared" si="23"/>
-        <v>302</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" s="7">
-        <v>1</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H52" s="5">
-        <v>39</v>
-      </c>
-      <c r="I52" s="1">
-        <f t="shared" si="21"/>
-        <v>39</v>
-      </c>
-      <c r="J52" s="5">
-        <v>39</v>
-      </c>
-      <c r="K52" s="5">
-        <f t="shared" si="22"/>
-        <v>1950</v>
-      </c>
-      <c r="L52" s="5">
-        <v>39</v>
-      </c>
-      <c r="M52" s="1">
-        <f t="shared" si="23"/>
-        <v>3900</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F53" s="7">
-        <v>1</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H53" s="5">
-        <v>0.71</v>
-      </c>
-      <c r="I53" s="1">
-        <f t="shared" si="21"/>
-        <v>0.71</v>
-      </c>
-      <c r="J53" s="5">
-        <v>3.21</v>
-      </c>
-      <c r="K53" s="5">
-        <f t="shared" si="22"/>
-        <v>160.5</v>
-      </c>
-      <c r="L53" s="5">
-        <v>0.51619999999999999</v>
-      </c>
-      <c r="M53" s="1">
-        <f t="shared" si="23"/>
-        <v>51.62</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F54" s="7">
-        <v>1</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H54" s="5">
-        <v>0.76</v>
-      </c>
-      <c r="I54" s="1">
-        <f t="shared" si="21"/>
-        <v>0.76</v>
-      </c>
-      <c r="J54" s="5">
-        <v>0.66300000000000003</v>
-      </c>
-      <c r="K54" s="5">
-        <f t="shared" si="22"/>
-        <v>33.15</v>
-      </c>
-      <c r="L54" s="5">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="M54" s="1">
-        <f t="shared" si="23"/>
-        <v>56.000000000000007</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B55" t="s">
-        <v>109</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F55" s="7">
-        <v>1</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H55" s="1">
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="I55" s="1">
-        <f t="shared" si="21"/>
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="J55" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="K55" s="1">
-        <f t="shared" si="22"/>
-        <v>375</v>
-      </c>
-      <c r="L55" s="1">
-        <v>6.9</v>
-      </c>
-      <c r="M55" s="1">
-        <f t="shared" si="23"/>
-        <v>690</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B56" s="13">
-        <v>132193</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D56" s="7"/>
-      <c r="F56" s="7">
-        <v>1</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="H56" s="1">
-        <v>6.12</v>
-      </c>
-      <c r="I56" s="1">
-        <f t="shared" si="21"/>
-        <v>6.12</v>
-      </c>
-      <c r="J56" s="1">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="K56" s="1">
-        <f t="shared" si="22"/>
-        <v>254.99999999999997</v>
-      </c>
-      <c r="L56" s="1">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="M56" s="1">
-        <f t="shared" si="23"/>
-        <v>484.99999999999994</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G58" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I58" s="1">
-        <f>SUM(I2:I56)</f>
-        <v>77.266800000000003</v>
-      </c>
-      <c r="K58" s="1">
-        <f>SUM(K2:K56)</f>
-        <v>3654.3500000000004</v>
-      </c>
-      <c r="M58" s="1">
-        <f>SUM(M2:M56)</f>
-        <v>6819.87</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G59" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="I59" s="1">
-        <f>I58/1</f>
-        <v>77.266800000000003</v>
-      </c>
-      <c r="K59" s="1">
-        <f>K58/50</f>
-        <v>73.087000000000003</v>
-      </c>
-      <c r="M59" s="1">
-        <f>M58/100</f>
+        <f>M48/100</f>
         <v>68.198700000000002</v>
       </c>
     </row>
@@ -2997,6 +2788,6 @@
     <sortCondition ref="A2:A52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="69" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>